<commit_message>
added some more sim files
</commit_message>
<xml_diff>
--- a/analysis/042114_chi-squared.xlsx
+++ b/analysis/042114_chi-squared.xlsx
@@ -398,10 +398,10 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="22.5703125"/>
     <col min="2" max="4" width="11.5703125"/>
@@ -414,7 +414,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="12.75">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +431,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -450,7 +450,7 @@
         <v>625.19236688211754</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -469,7 +469,7 @@
         <v>362.13991769547323</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="12.75">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -488,7 +488,7 @@
         <v>302.06933619994629</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="12.75">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -507,7 +507,7 @@
         <v>191.94863587867707</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="12.75">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -526,7 +526,7 @@
         <v>80.261593341260394</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="12.75">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -561,7 +561,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1025" width="11.5703125"/>
   </cols>
@@ -580,7 +580,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1025" width="11.5703125"/>
   </cols>

</xml_diff>